<commit_message>
P2-L8 and demo minor improv.
</commit_message>
<xml_diff>
--- a/LectureNotes-part2-PSB/P2-L8 - mle-demo.xlsx
+++ b/LectureNotes-part2-PSB/P2-L8 - mle-demo.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GDrives\prak-SMAIL-IITM-UCD\courses_mine\MUDE-working-psb\psb-notes\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D0A1F6C9-A0FA-4031-BA24-A38B08CFC005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{237F22CE-8191-4945-B205-642FC977B670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{74562D28-3343-4C62-B309-85AC3405D8FF}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{74562D28-3343-4C62-B309-85AC3405D8FF}"/>
   </bookViews>
   <sheets>
     <sheet name="mle-demo-L8" sheetId="2" r:id="rId1"/>
@@ -634,61 +634,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1"/>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" sz="1200"/>
-              <a:t>MLE</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" sz="1200" baseline="0"/>
-              <a:t> example</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US" sz="1200"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1"/>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout>
         <c:manualLayout>
@@ -696,9 +642,9 @@
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
           <c:x val="0.16822802241619547"/>
-          <c:y val="0.13004629629629633"/>
+          <c:y val="6.0798640784674951E-2"/>
           <c:w val="0.7647120705253635"/>
-          <c:h val="0.75792395742198881"/>
+          <c:h val="0.82717151114922249"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1443,9 +1389,9 @@
         <c:manualLayout>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.64348421574875514"/>
+          <c:x val="0.53466393715923832"/>
           <c:y val="0.7274300087489064"/>
-          <c:w val="0.27330071487764013"/>
+          <c:w val="0.382120857075267"/>
           <c:h val="0.12905147273257508"/>
         </c:manualLayout>
       </c:layout>
@@ -1492,10 +1438,7 @@
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:solidFill>
       <a:round/>
     </a:ln>
@@ -2527,14 +2470,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CC61411-91D7-47A9-AF8A-2A241ADDAA7B}">
   <dimension ref="B1:T105"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
-      <selection activeCell="O7" sqref="O7"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="4.28515625" customWidth="1"/>
-    <col min="2" max="2" width="9.85546875" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
     <col min="3" max="8" width="6.42578125" style="1" customWidth="1"/>
     <col min="10" max="11" width="5.28515625" customWidth="1"/>
     <col min="12" max="13" width="8.28515625" customWidth="1"/>

</xml_diff>